<commit_message>
Add Elvis test document (longest article in English apparently)
</commit_message>
<xml_diff>
--- a/Compare_Tests.xlsx
+++ b/Compare_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/project-symmetry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60743846-79B9-E84D-9F67-6B77AB34D399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE49FAA3-6FE9-274B-A2D2-1A4DF162A861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{C6D50D6E-BAF6-1D48-8564-4D25AB3A0685}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{C6D50D6E-BAF6-1D48-8564-4D25AB3A0685}"/>
   </bookViews>
   <sheets>
     <sheet name="BLEU Score" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Lang 1</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>[Visual Studio Code, Compare Tool, Excel, Finder]</t>
+  </si>
+  <si>
+    <t>Elvis Presley (Largest in English src: https://diff.wikimedia.org/2016/05/12/rock-n-scroll-english-wikipedias-longest-featured-articles/)</t>
   </si>
 </sst>
 </file>
@@ -453,12 +456,12 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="30.1640625" customWidth="1"/>
@@ -589,6 +592,15 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>589</v>
+      </c>
       <c r="F3">
         <v>5.0000000000000001E-4</v>
       </c>

</xml_diff>

<commit_message>
Add tests for Elvis article
</commit_message>
<xml_diff>
--- a/Compare_Tests.xlsx
+++ b/Compare_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/project-symmetry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D8415-AC8B-DD4D-9B6D-3A054C8FCB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E65CD5-588C-244E-9615-AFBDC88179FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{C6D50D6E-BAF6-1D48-8564-4D25AB3A0685}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Lang 1</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Num Iterations O(m*n)</t>
   </si>
   <si>
-    <t>Elvis Presley (Largest in English src: https://diff.wikimedia.org/2016/05/12/rock-n-scroll-english-wikipedias-longest-featured-articles/)</t>
-  </si>
-  <si>
     <t>Boris Johnson</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Visual Studio Code</t>
+  </si>
+  <si>
+    <t>Elvis Presley</t>
   </si>
 </sst>
 </file>
@@ -143,8 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,278 +464,309 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB9EBA7-2BE5-AA44-97C0-CA3360606022}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" customWidth="1"/>
-    <col min="7" max="7" width="27.83203125" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" customWidth="1"/>
-    <col min="11" max="11" width="25.5" customWidth="1"/>
-    <col min="12" max="12" width="25.83203125" customWidth="1"/>
-    <col min="13" max="13" width="29.1640625" customWidth="1"/>
-    <col min="14" max="14" width="29.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.1640625" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" customWidth="1"/>
-    <col min="18" max="18" width="45.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="29.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" style="1" customWidth="1"/>
     <col min="19" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>673</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>414</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <f>D2*E2</f>
         <v>278622</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <f>G2 * F2 / 60</f>
         <v>2.32185</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <f>G2 * F2</f>
         <v>139.31100000000001</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>92</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>94.3</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>89.48</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>90.82</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>92.36</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <f>AVERAGE(J2, K2, L2, M2, N2)</f>
         <v>91.792000000000002</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <f xml:space="preserve"> O2 / 60</f>
         <v>1.5298666666666667</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <f xml:space="preserve"> O2 / G2</f>
         <v>3.2944993575525263E-4</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>993</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>366</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <f>0.0006</f>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <f t="shared" ref="G3:G10" si="0">D3*E3</f>
         <v>363438</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <f t="shared" ref="H3:H10" si="1">G3 * F3 / 60</f>
         <v>3.6343799999999997</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <f>G3 * F3</f>
         <v>218.06279999999998</v>
       </c>
+      <c r="J3" s="1">
+        <v>112.99</v>
+      </c>
+      <c r="K3" s="1">
+        <v>112.11</v>
+      </c>
+      <c r="L3" s="1">
+        <v>112.5</v>
+      </c>
+      <c r="M3" s="1">
+        <v>110.5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>110.15</v>
+      </c>
+      <c r="O3" s="1">
+        <f>AVERAGE(J3, K3, L3, M3, N3)</f>
+        <v>111.65</v>
+      </c>
+      <c r="P3" s="1">
+        <f xml:space="preserve"> O3 / 60</f>
+        <v>1.8608333333333333</v>
+      </c>
+      <c r="Q3" s="1">
+        <f xml:space="preserve"> O3 / G3</f>
+        <v>3.0720508037134257E-4</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>216</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <f>G4 * F4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G5">
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <f>G5 * F5 / 60</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G6">
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <f>G6 * F6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G7">
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <f>G7 * F7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G8">
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <f>G8 * F8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <f>G9 * F9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add error calculation (est - actual)
</commit_message>
<xml_diff>
--- a/Compare_Tests.xlsx
+++ b/Compare_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/project-symmetry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E65CD5-588C-244E-9615-AFBDC88179FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7EFB9-12BE-E648-9AB4-D4E88C5D4F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{C6D50D6E-BAF6-1D48-8564-4D25AB3A0685}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Lang 1</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Elvis Presley</t>
+  </si>
+  <si>
+    <t>Est - Actual</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB9EBA7-2BE5-AA44-97C0-CA3360606022}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,11 +490,12 @@
     <col min="16" max="16" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.33203125" style="1" customWidth="1"/>
-    <col min="19" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -544,10 +548,13 @@
         <v>21</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -575,8 +582,8 @@
         <v>2.32185</v>
       </c>
       <c r="I2" s="1">
-        <f>G2 * F2</f>
-        <v>139.31100000000001</v>
+        <f>ROUNDUP(G2 * F2, 2)</f>
+        <v>139.32</v>
       </c>
       <c r="J2" s="1">
         <v>92</v>
@@ -605,11 +612,15 @@
         <f xml:space="preserve"> O2 / G2</f>
         <v>3.2944993575525263E-4</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="1">
+        <f>I2 - O2</f>
+        <v>47.527999999999992</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -626,8 +637,8 @@
         <v>366</v>
       </c>
       <c r="F3" s="1">
-        <f>0.0006</f>
-        <v>5.9999999999999995E-4</v>
+        <f>0.0005</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G10" si="0">D3*E3</f>
@@ -635,11 +646,11 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H10" si="1">G3 * F3 / 60</f>
-        <v>3.6343799999999997</v>
+        <v>3.0286499999999998</v>
       </c>
       <c r="I3" s="1">
-        <f>G3 * F3</f>
-        <v>218.06279999999998</v>
+        <f t="shared" ref="I3:I10" si="2">ROUNDUP(G3 * F3, 2)</f>
+        <v>181.72</v>
       </c>
       <c r="J3" s="1">
         <v>112.99</v>
@@ -668,11 +679,15 @@
         <f xml:space="preserve"> O3 / G3</f>
         <v>3.0720508037134257E-4</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="1">
+        <f>I3 - O3</f>
+        <v>70.069999999999993</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -682,6 +697,10 @@
       <c r="D4" s="1">
         <v>216</v>
       </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F10" si="3">0.0005</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -691,11 +710,31 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f>G4 * F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="e">
+        <f t="shared" ref="O4:O11" si="4">AVERAGE(J4, K4, L4, M4, N4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" s="1" t="e">
+        <f t="shared" ref="P4:P11" si="5" xml:space="preserve"> O4 / 60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q4" s="1" t="e">
+        <f t="shared" ref="Q4:Q11" si="6" xml:space="preserve"> O4 / G4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R4" s="1" t="e">
+        <f t="shared" ref="R4:R11" si="7">I4 - O4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F5" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -704,8 +743,32 @@
         <f>G5 * F5 / 60</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q5" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R5" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -715,11 +778,31 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f>G6 * F6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q6" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R6" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F7" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -729,11 +812,31 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f>G7 * F7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q7" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R7" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -743,11 +846,31 @@
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f>G8 * F8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q8" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R8" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F9" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -757,11 +880,31 @@
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <f>G9 * F9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F10" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -769,6 +912,44 @@
       <c r="H10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q10" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R10" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O11" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q11" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R11" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add section test template
</commit_message>
<xml_diff>
--- a/Compare_Tests.xlsx
+++ b/Compare_Tests.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/project-symmetry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7EFB9-12BE-E648-9AB4-D4E88C5D4F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC872F51-4D19-F043-B600-5A541439B44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{C6D50D6E-BAF6-1D48-8564-4D25AB3A0685}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{C6D50D6E-BAF6-1D48-8564-4D25AB3A0685}"/>
   </bookViews>
   <sheets>
-    <sheet name="BLEU Score" sheetId="1" r:id="rId1"/>
+    <sheet name="Whole Article BLEU Score" sheetId="1" r:id="rId1"/>
+    <sheet name="Section BLEU Score" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Lang 1</t>
   </si>
@@ -111,6 +112,15 @@
   </si>
   <si>
     <t>Est - Actual</t>
+  </si>
+  <si>
+    <t>Section Name</t>
+  </si>
+  <si>
+    <t>Sentences Section 1</t>
+  </si>
+  <si>
+    <t>Sentences Section 2</t>
   </si>
 </sst>
 </file>
@@ -467,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB9EBA7-2BE5-AA44-97C0-CA3360606022}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -958,4 +968,98 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2240BB-A368-9742-B5AB-248B9358CFD7}">
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="30.83203125" customWidth="1"/>
+    <col min="12" max="13" width="27.5" customWidth="1"/>
+    <col min="14" max="14" width="26.83203125" customWidth="1"/>
+    <col min="15" max="15" width="32.83203125" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="19" width="12.5" customWidth="1"/>
+    <col min="20" max="20" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>